<commit_message>
Added Testcases -Fourth commit
</commit_message>
<xml_diff>
--- a/TestData/TestData.xlsx
+++ b/TestData/TestData.xlsx
@@ -8,13 +8,15 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\AutomationTraining\CreatioTestNGFramework\TestData\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{95F7D43B-0F79-49E4-A25B-B54B1B535102}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CF3D9B83-FA17-45DB-B39D-93A2F96E3754}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="verifyLoginPageLogoAndHeader" sheetId="3" r:id="rId1"/>
-    <sheet name="verifyLoginWithValidCredentials" sheetId="4" r:id="rId2"/>
+    <sheet name="verifyLoginWithValidCredentials" sheetId="4" r:id="rId1"/>
+    <sheet name="verifyLoginInvalidCredentials" sheetId="6" r:id="rId2"/>
+    <sheet name="verifyForgotLoginFeature" sheetId="8" r:id="rId3"/>
+    <sheet name="verifyLoginPageLogoAndHeader" sheetId="3" r:id="rId4"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -26,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="8">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="13">
   <si>
     <t>LoginHeader</t>
   </si>
@@ -50,6 +52,21 @@
   </si>
   <si>
     <t>header</t>
+  </si>
+  <si>
+    <t>errorMessage</t>
+  </si>
+  <si>
+    <t>Invalid email or password</t>
+  </si>
+  <si>
+    <t>Harish</t>
+  </si>
+  <si>
+    <t>null</t>
+  </si>
+  <si>
+    <t>Almost done!</t>
   </si>
 </sst>
 </file>
@@ -383,6 +400,132 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DAFD94C8-0339-4A8B-9759-038D879CE161}">
+  <dimension ref="A1:C2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C1" sqref="C1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="14" customWidth="1"/>
+    <col min="2" max="2" width="11.88671875" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A1" t="s">
+        <v>5</v>
+      </c>
+      <c r="B1" t="s">
+        <v>6</v>
+      </c>
+      <c r="C1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A2" t="s">
+        <v>2</v>
+      </c>
+      <c r="B2" t="s">
+        <v>3</v>
+      </c>
+      <c r="C2" s="2" t="s">
+        <v>4</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D741E3AE-6EE0-4D9B-81FF-7F4318D9B464}">
+  <dimension ref="A1:C2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:C1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="14" customWidth="1"/>
+    <col min="2" max="2" width="11.88671875" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A1" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A2" t="s">
+        <v>2</v>
+      </c>
+      <c r="B2" t="s">
+        <v>10</v>
+      </c>
+      <c r="C2" t="s">
+        <v>9</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2D9F7055-799C-46D0-80E3-3B2F5C9F445C}">
+  <dimension ref="A1:C2"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C2" sqref="C2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="28.33203125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="11.88671875" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A1" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A2" t="s">
+        <v>2</v>
+      </c>
+      <c r="B2" t="s">
+        <v>11</v>
+      </c>
+      <c r="C2" s="2" t="s">
+        <v>12</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F4ECE66A-8654-47FB-B225-99390EAD3D2D}">
   <dimension ref="A1:A2"/>
   <sheetViews>
@@ -409,46 +552,4 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
 </worksheet>
-</file>
-
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DAFD94C8-0339-4A8B-9759-038D879CE161}">
-  <dimension ref="A1:C2"/>
-  <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C1" sqref="C1"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
-  <cols>
-    <col min="1" max="1" width="14" customWidth="1"/>
-    <col min="2" max="2" width="11.88671875" bestFit="1" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A1" t="s">
-        <v>5</v>
-      </c>
-      <c r="B1" t="s">
-        <v>6</v>
-      </c>
-      <c r="C1" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A2" t="s">
-        <v>2</v>
-      </c>
-      <c r="B2" t="s">
-        <v>3</v>
-      </c>
-      <c r="C2" s="2" t="s">
-        <v>4</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId1"/>
-</worksheet>
 </file>
</xml_diff>